<commit_message>
data cleanup continued in multi dfs, major code refactoring taking place contiued
</commit_message>
<xml_diff>
--- a/TEST_TEMP_TO_BE_REMOVED.xlsx
+++ b/TEST_TEMP_TO_BE_REMOVED.xlsx
@@ -14,12 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <si>
+    <t>season_ending_year</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>blk_per_game</t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>ABA</t>
+  </si>
+  <si>
+    <t>BAA</t>
   </si>
 </sst>
 </file>
@@ -377,41 +389,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2">
-        <v>99</v>
-      </c>
-      <c r="B2">
-        <v>200</v>
+        <v>1971</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3">
-        <v>199</v>
+        <v>1975</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4">
-        <v>299</v>
+        <v>1974</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5">
-        <v>399</v>
+        <v>1972</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>